<commit_message>
reject estimator dan rab
</commit_message>
<xml_diff>
--- a/public/samplerecord.xlsx
+++ b/public/samplerecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\solan-app-final\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E80E87B-8884-45A7-B135-0B6F73452B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1F0F52-EECA-4C79-93B6-C8F50EBD4904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">Tanggal : </t>
   </si>
   <si>
-    <t>SAMPLE RECORD</t>
-  </si>
-  <si>
     <t>Nama Order:</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Nama&amp;Paraf :</t>
+  </si>
+  <si>
+    <t>SPK RECORD</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -577,6 +577,93 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -628,94 +715,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,175 +1068,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="80"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+    <row r="1" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="45"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="86"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="83"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="48"/>
+    </row>
+    <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="87" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="E4" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="2"/>
       <c r="I4" s="37"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="62"/>
-    </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="60" t="s">
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="62"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="73" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="60"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="8"/>
       <c r="J6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="60"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="66" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="72" t="s">
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="77"/>
+      <c r="H7" s="71"/>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="74" t="s">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="63"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="75"/>
+      <c r="H8" s="69"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="8"/>
       <c r="D9" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="8"/>
       <c r="G9" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="8"/>
       <c r="J9" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="14"/>
       <c r="D10" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="11"/>
@@ -1247,9 +1246,9 @@
       <c r="J10" s="22"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="8"/>
@@ -1262,76 +1261,75 @@
       <c r="J11" s="22"/>
       <c r="K11" s="42"/>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="49" t="s">
+      <c r="D12" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="E12" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="F12" s="82"/>
+      <c r="G12" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="53"/>
-      <c r="G12" s="52" t="s">
+      <c r="H12" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="52" t="s">
+      <c r="I12" s="82"/>
+      <c r="J12" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="53"/>
-      <c r="J12" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="53"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="55"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="57"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="82"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="74"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="84"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="84"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="76"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="86"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="K16" s="4"/>
-      <c r="M16" s="89"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1456,106 +1454,106 @@
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="40" t="s">
         <v>19</v>
-      </c>
-      <c r="B45" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I45" s="40" t="s">
-        <v>20</v>
       </c>
       <c r="J45" s="41"/>
       <c r="K45" s="4"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>22</v>
-      </c>
       <c r="C46" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="32" t="s">
-        <v>22</v>
-      </c>
       <c r="E46" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="32" t="s">
-        <v>22</v>
-      </c>
       <c r="G46" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="32" t="s">
         <v>21</v>
-      </c>
-      <c r="H46" s="32" t="s">
-        <v>22</v>
       </c>
       <c r="I46" s="6"/>
       <c r="K46" s="4"/>
     </row>
     <row r="47" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="34" t="s">
-        <v>24</v>
-      </c>
       <c r="C47" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D47" s="34" t="s">
-        <v>24</v>
-      </c>
       <c r="E47" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="34" t="s">
-        <v>24</v>
-      </c>
       <c r="G47" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="34" t="s">
         <v>23</v>
-      </c>
-      <c r="H47" s="34" t="s">
-        <v>24</v>
       </c>
       <c r="I47" s="6"/>
       <c r="K47" s="4"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="34"/>
       <c r="C48" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" s="34"/>
       <c r="E48" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" s="34"/>
       <c r="G48" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H48" s="34"/>
       <c r="I48" s="6"/>
@@ -1564,59 +1562,59 @@
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C49" s="30"/>
       <c r="D49" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E49" s="30"/>
       <c r="F49" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G49" s="30"/>
       <c r="H49" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I49" s="6"/>
       <c r="K49" s="4"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
-      <c r="B50" s="58" t="s">
-        <v>26</v>
+      <c r="B50" s="87" t="s">
+        <v>25</v>
       </c>
       <c r="C50" s="30"/>
-      <c r="D50" s="58" t="s">
-        <v>26</v>
+      <c r="D50" s="87" t="s">
+        <v>25</v>
       </c>
       <c r="E50" s="30"/>
-      <c r="F50" s="58" t="s">
-        <v>26</v>
+      <c r="F50" s="87" t="s">
+        <v>25</v>
       </c>
       <c r="G50" s="30"/>
-      <c r="H50" s="58" t="s">
-        <v>26</v>
+      <c r="H50" s="87" t="s">
+        <v>25</v>
       </c>
       <c r="I50" s="6"/>
       <c r="K50" s="4"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
-      <c r="B51" s="59"/>
+      <c r="B51" s="88"/>
       <c r="C51" s="31"/>
-      <c r="D51" s="59"/>
+      <c r="D51" s="88"/>
       <c r="E51" s="31"/>
-      <c r="F51" s="59"/>
+      <c r="F51" s="88"/>
       <c r="G51" s="31"/>
-      <c r="H51" s="59"/>
+      <c r="H51" s="88"/>
       <c r="I51" s="7"/>
       <c r="J51" s="17"/>
       <c r="K51" s="5"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
@@ -1627,7 +1625,7 @@
       <c r="H52" s="25"/>
       <c r="I52" s="25"/>
       <c r="J52" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K52" s="26"/>
     </row>
@@ -1646,12 +1644,17 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="E12:F15"/>
+    <mergeCell ref="J12:K15"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:I15"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="A6:C8"/>
     <mergeCell ref="G6:H6"/>
@@ -1663,17 +1666,12 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="E12:F15"/>
-    <mergeCell ref="J12:K15"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:I15"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="10000" orientation="portrait" r:id="rId1"/>

</xml_diff>